<commit_message>
CAN ids assigned, added CAN matrix cycle to ML SL
</commit_message>
<xml_diff>
--- a/CANmatrix/CAN_matrix.xlsx
+++ b/CANmatrix/CAN_matrix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Temp\LOCAL\Studie\DS\ProjectRepo\DS_MinorProject\CANmatrix\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{19BF9856-FF91-4160-9CD7-493B05A881AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0B9D859-9BE1-4438-81C5-FF4867D0AB9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2535" yWindow="1920" windowWidth="21600" windowHeight="11385" xr2:uid="{C08CBC26-4CD9-498F-B1F0-48518EE41BF6}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C08CBC26-4CD9-498F-B1F0-48518EE41BF6}"/>
   </bookViews>
   <sheets>
     <sheet name="Messages" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="63">
   <si>
     <t>Name</t>
   </si>
@@ -223,6 +223,9 @@
   </si>
   <si>
     <t>Sparse</t>
+  </si>
+  <si>
+    <t>ID (Dec)</t>
   </si>
 </sst>
 </file>
@@ -646,7 +649,7 @@
   <dimension ref="A1:N16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -866,6 +869,33 @@
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>62</v>
+      </c>
+      <c r="B14">
+        <v>11</v>
+      </c>
+      <c r="C14">
+        <v>12</v>
+      </c>
+      <c r="D14">
+        <v>13</v>
+      </c>
+      <c r="E14">
+        <v>14</v>
+      </c>
+      <c r="G14">
+        <v>26</v>
+      </c>
+      <c r="H14">
+        <v>37</v>
+      </c>
+      <c r="I14">
+        <v>48</v>
+      </c>
+      <c r="J14">
+        <v>59</v>
+      </c>
       <c r="M14" s="7" t="s">
         <v>33</v>
       </c>

</xml_diff>

<commit_message>
working version of complete matrix cycle and HANtune project dash
</commit_message>
<xml_diff>
--- a/CANmatrix/CAN_matrix.xlsx
+++ b/CANmatrix/CAN_matrix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Temp\LOCAL\Studie\DS\ProjectRepo\DS_MinorProject\CANmatrix\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0B9D859-9BE1-4438-81C5-FF4867D0AB9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{701C8618-FE3F-4AB5-8DB2-0B9AF922975A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C08CBC26-4CD9-498F-B1F0-48518EE41BF6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C08CBC26-4CD9-498F-B1F0-48518EE41BF6}"/>
   </bookViews>
   <sheets>
     <sheet name="Messages" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="65">
   <si>
     <t>Name</t>
   </si>
@@ -226,6 +226,12 @@
   </si>
   <si>
     <t>ID (Dec)</t>
+  </si>
+  <si>
+    <t>Slot number</t>
+  </si>
+  <si>
+    <t>Slot time</t>
   </si>
 </sst>
 </file>
@@ -254,7 +260,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -306,6 +312,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -322,7 +340,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -332,6 +350,8 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -649,24 +669,24 @@
   <dimension ref="A1:N16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="39.42578125" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" customWidth="1"/>
-    <col min="3" max="3" width="20.7109375" customWidth="1"/>
+    <col min="1" max="1" width="39.44140625" customWidth="1"/>
+    <col min="2" max="2" width="10.88671875" customWidth="1"/>
+    <col min="3" max="3" width="20.6640625" customWidth="1"/>
     <col min="4" max="4" width="23" customWidth="1"/>
-    <col min="5" max="5" width="21.85546875" customWidth="1"/>
+    <col min="5" max="5" width="21.88671875" customWidth="1"/>
     <col min="6" max="6" width="21" customWidth="1"/>
-    <col min="7" max="7" width="22.5703125" customWidth="1"/>
-    <col min="8" max="8" width="20.5703125" customWidth="1"/>
-    <col min="9" max="9" width="19.85546875" customWidth="1"/>
-    <col min="10" max="10" width="22.42578125" customWidth="1"/>
+    <col min="7" max="7" width="22.5546875" customWidth="1"/>
+    <col min="8" max="8" width="20.5546875" customWidth="1"/>
+    <col min="9" max="9" width="19.88671875" customWidth="1"/>
+    <col min="10" max="10" width="22.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -698,7 +718,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -720,8 +740,11 @@
       <c r="G2" s="3" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J2" s="9" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -749,8 +772,11 @@
       <c r="I3" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J3" s="9" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -763,19 +789,28 @@
       <c r="D4" s="6" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J4" s="9" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>40</v>
       </c>
       <c r="B5" t="s">
         <v>37</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="D5" s="7" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J5" s="9" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>39</v>
       </c>
@@ -788,8 +823,11 @@
       <c r="D6" s="1" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="J6" s="9" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>25</v>
       </c>
@@ -827,7 +865,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>48</v>
       </c>
@@ -868,7 +906,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>62</v>
       </c>
@@ -903,7 +941,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="M15" s="1" t="s">
         <v>34</v>
       </c>
@@ -911,7 +949,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="M16" s="3" t="s">
         <v>35</v>
       </c>
@@ -933,19 +971,19 @@
       <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
-    <col min="2" max="2" width="10.28515625" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" customWidth="1"/>
-    <col min="4" max="4" width="10.5703125" customWidth="1"/>
+    <col min="2" max="2" width="10.33203125" customWidth="1"/>
+    <col min="3" max="3" width="11.88671875" customWidth="1"/>
+    <col min="4" max="4" width="10.5546875" customWidth="1"/>
     <col min="5" max="6" width="11" customWidth="1"/>
-    <col min="7" max="7" width="10.42578125" customWidth="1"/>
-    <col min="8" max="8" width="11.42578125" customWidth="1"/>
-    <col min="10" max="10" width="10.5703125" customWidth="1"/>
+    <col min="7" max="7" width="10.44140625" customWidth="1"/>
+    <col min="8" max="8" width="11.44140625" customWidth="1"/>
+    <col min="10" max="10" width="10.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>25</v>
       </c>
@@ -983,7 +1021,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>48</v>
       </c>
@@ -1024,7 +1062,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="M3" s="7" t="s">
         <v>33</v>
       </c>
@@ -1032,7 +1070,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="M4" s="1" t="s">
         <v>34</v>
       </c>
@@ -1040,7 +1078,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="M5" s="3" t="s">
         <v>35</v>
       </c>

</xml_diff>

<commit_message>
Added a combined model of kinematic model, motor model and tt can model
</commit_message>
<xml_diff>
--- a/CANmatrix/CAN_matrix.xlsx
+++ b/CANmatrix/CAN_matrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Temp\LOCAL\Studie\DS\ProjectRepo\DS_MinorProject\CANmatrix\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{701C8618-FE3F-4AB5-8DB2-0B9AF922975A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF75B925-BD96-4092-99B8-9105D9736B86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C08CBC26-4CD9-498F-B1F0-48518EE41BF6}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="65">
   <si>
     <t>Name</t>
   </si>
@@ -668,8 +668,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB598DAD-510F-4626-AEEC-E2A56A0E037C}">
   <dimension ref="A1:N16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -968,7 +968,7 @@
   <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1063,6 +1063,33 @@
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3">
+        <v>11</v>
+      </c>
+      <c r="C3">
+        <v>12</v>
+      </c>
+      <c r="D3">
+        <v>13</v>
+      </c>
+      <c r="E3">
+        <v>14</v>
+      </c>
+      <c r="G3">
+        <v>26</v>
+      </c>
+      <c r="H3">
+        <v>37</v>
+      </c>
+      <c r="I3">
+        <v>48</v>
+      </c>
+      <c r="J3">
+        <v>59</v>
+      </c>
       <c r="M3" s="7" t="s">
         <v>33</v>
       </c>

</xml_diff>

<commit_message>
minor HT dash update + update matrix cycle, added IO and algorithm to sparse slots
</commit_message>
<xml_diff>
--- a/CANmatrix/CAN_matrix.xlsx
+++ b/CANmatrix/CAN_matrix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Temp\LOCAL\Studie\DS\ProjectRepo\DS_MinorProject\CANmatrix\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF75B925-BD96-4092-99B8-9105D9736B86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F774AC57-DBC9-44A0-B0C1-CEB093A94FD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C08CBC26-4CD9-498F-B1F0-48518EE41BF6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C08CBC26-4CD9-498F-B1F0-48518EE41BF6}"/>
   </bookViews>
   <sheets>
     <sheet name="Messages" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="66">
   <si>
     <t>Name</t>
   </si>
@@ -232,6 +232,9 @@
   </si>
   <si>
     <t>Slot time</t>
+  </si>
+  <si>
+    <t>IO  + Control execution</t>
   </si>
 </sst>
 </file>
@@ -668,25 +671,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB598DAD-510F-4626-AEEC-E2A56A0E037C}">
   <dimension ref="A1:N16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:J6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.44140625" customWidth="1"/>
-    <col min="2" max="2" width="10.88671875" customWidth="1"/>
-    <col min="3" max="3" width="20.6640625" customWidth="1"/>
+    <col min="1" max="1" width="39.42578125" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" customWidth="1"/>
+    <col min="3" max="3" width="20.7109375" customWidth="1"/>
     <col min="4" max="4" width="23" customWidth="1"/>
-    <col min="5" max="5" width="21.88671875" customWidth="1"/>
+    <col min="5" max="5" width="21.85546875" customWidth="1"/>
     <col min="6" max="6" width="21" customWidth="1"/>
-    <col min="7" max="7" width="22.5546875" customWidth="1"/>
-    <col min="8" max="8" width="20.5546875" customWidth="1"/>
-    <col min="9" max="9" width="19.88671875" customWidth="1"/>
-    <col min="10" max="10" width="22.44140625" customWidth="1"/>
+    <col min="7" max="7" width="22.5703125" customWidth="1"/>
+    <col min="8" max="8" width="20.5703125" customWidth="1"/>
+    <col min="9" max="9" width="19.85546875" customWidth="1"/>
+    <col min="10" max="10" width="22.42578125" customWidth="1"/>
+    <col min="11" max="11" width="22.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -718,7 +722,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -744,7 +748,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -776,7 +780,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -793,7 +797,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>40</v>
       </c>
@@ -810,7 +814,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>39</v>
       </c>
@@ -827,7 +831,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>25</v>
       </c>
@@ -865,7 +869,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>48</v>
       </c>
@@ -882,7 +886,7 @@
         <v>51</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="G13" s="4" t="s">
         <v>52</v>
@@ -897,7 +901,7 @@
         <v>50</v>
       </c>
       <c r="K13" s="8" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="M13" s="4" t="s">
         <v>32</v>
@@ -906,7 +910,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>62</v>
       </c>
@@ -941,7 +945,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="M15" s="1" t="s">
         <v>34</v>
       </c>
@@ -949,7 +953,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="M16" s="3" t="s">
         <v>35</v>
       </c>
@@ -968,22 +972,22 @@
   <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
-    <col min="2" max="2" width="10.33203125" customWidth="1"/>
-    <col min="3" max="3" width="11.88671875" customWidth="1"/>
-    <col min="4" max="4" width="10.5546875" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" customWidth="1"/>
+    <col min="4" max="4" width="10.5703125" customWidth="1"/>
     <col min="5" max="6" width="11" customWidth="1"/>
-    <col min="7" max="7" width="10.44140625" customWidth="1"/>
-    <col min="8" max="8" width="11.44140625" customWidth="1"/>
-    <col min="10" max="10" width="10.5546875" customWidth="1"/>
+    <col min="7" max="7" width="10.42578125" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" customWidth="1"/>
+    <col min="10" max="10" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>25</v>
       </c>
@@ -1021,7 +1025,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>48</v>
       </c>
@@ -1062,7 +1066,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>62</v>
       </c>
@@ -1097,7 +1101,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="M4" s="1" t="s">
         <v>34</v>
       </c>
@@ -1105,7 +1109,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="M5" s="3" t="s">
         <v>35</v>
       </c>

</xml_diff>

<commit_message>
Updated Combined model membership with buttonpress on CAN
</commit_message>
<xml_diff>
--- a/CANmatrix/CAN_matrix.xlsx
+++ b/CANmatrix/CAN_matrix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Temp\LOCAL\Studie\DS\ProjectRepo\DS_MinorProject\CANmatrix\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F774AC57-DBC9-44A0-B0C1-CEB093A94FD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CE82F07-08B0-4EC7-8144-46D92626BCAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C08CBC26-4CD9-498F-B1F0-48518EE41BF6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C08CBC26-4CD9-498F-B1F0-48518EE41BF6}"/>
   </bookViews>
   <sheets>
     <sheet name="Messages" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="67">
   <si>
     <t>Name</t>
   </si>
@@ -235,6 +235,9 @@
   </si>
   <si>
     <t>IO  + Control execution</t>
+  </si>
+  <si>
+    <t>Button press</t>
   </si>
 </sst>
 </file>
@@ -263,7 +266,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -327,6 +330,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -343,7 +352,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -355,6 +364,7 @@
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -671,26 +681,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB598DAD-510F-4626-AEEC-E2A56A0E037C}">
   <dimension ref="A1:N16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="39.42578125" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" customWidth="1"/>
-    <col min="3" max="3" width="20.7109375" customWidth="1"/>
+    <col min="1" max="1" width="39.44140625" customWidth="1"/>
+    <col min="2" max="2" width="10.88671875" customWidth="1"/>
+    <col min="3" max="3" width="20.6640625" customWidth="1"/>
     <col min="4" max="4" width="23" customWidth="1"/>
-    <col min="5" max="5" width="21.85546875" customWidth="1"/>
+    <col min="5" max="5" width="21.88671875" customWidth="1"/>
     <col min="6" max="6" width="21" customWidth="1"/>
-    <col min="7" max="7" width="22.5703125" customWidth="1"/>
-    <col min="8" max="8" width="20.5703125" customWidth="1"/>
-    <col min="9" max="9" width="19.85546875" customWidth="1"/>
-    <col min="10" max="10" width="22.42578125" customWidth="1"/>
-    <col min="11" max="11" width="22.7109375" customWidth="1"/>
+    <col min="7" max="7" width="22.5546875" customWidth="1"/>
+    <col min="8" max="8" width="20.5546875" customWidth="1"/>
+    <col min="9" max="9" width="19.88671875" customWidth="1"/>
+    <col min="10" max="10" width="22.44140625" customWidth="1"/>
+    <col min="11" max="11" width="22.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -722,7 +732,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -744,11 +754,14 @@
       <c r="G2" s="3" t="s">
         <v>17</v>
       </c>
+      <c r="H2" s="11" t="s">
+        <v>66</v>
+      </c>
       <c r="J2" s="9" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>20</v>
       </c>
@@ -780,7 +793,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -797,7 +810,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>40</v>
       </c>
@@ -814,7 +827,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>39</v>
       </c>
@@ -831,7 +844,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>25</v>
       </c>
@@ -869,7 +882,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>48</v>
       </c>
@@ -910,7 +923,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>62</v>
       </c>
@@ -945,7 +958,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="M15" s="1" t="s">
         <v>34</v>
       </c>
@@ -953,7 +966,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="M16" s="3" t="s">
         <v>35</v>
       </c>
@@ -975,19 +988,19 @@
       <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
-    <col min="2" max="2" width="10.28515625" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" customWidth="1"/>
-    <col min="4" max="4" width="10.5703125" customWidth="1"/>
+    <col min="2" max="2" width="10.33203125" customWidth="1"/>
+    <col min="3" max="3" width="11.88671875" customWidth="1"/>
+    <col min="4" max="4" width="10.5546875" customWidth="1"/>
     <col min="5" max="6" width="11" customWidth="1"/>
-    <col min="7" max="7" width="10.42578125" customWidth="1"/>
-    <col min="8" max="8" width="11.42578125" customWidth="1"/>
-    <col min="10" max="10" width="10.5703125" customWidth="1"/>
+    <col min="7" max="7" width="10.44140625" customWidth="1"/>
+    <col min="8" max="8" width="11.44140625" customWidth="1"/>
+    <col min="10" max="10" width="10.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>25</v>
       </c>
@@ -1025,7 +1038,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>48</v>
       </c>
@@ -1066,7 +1079,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>62</v>
       </c>
@@ -1101,7 +1114,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="M4" s="1" t="s">
         <v>34</v>
       </c>
@@ -1109,7 +1122,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="M5" s="3" t="s">
         <v>35</v>
       </c>

</xml_diff>

<commit_message>
Added fault checks and added CAN data
</commit_message>
<xml_diff>
--- a/CANmatrix/CAN_matrix.xlsx
+++ b/CANmatrix/CAN_matrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Temp\LOCAL\Studie\DS\ProjectRepo\DS_MinorProject\CANmatrix\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CE82F07-08B0-4EC7-8144-46D92626BCAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B605BA7-A9E7-42E5-9274-CB7B0E418458}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C08CBC26-4CD9-498F-B1F0-48518EE41BF6}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="67">
   <si>
     <t>Name</t>
   </si>
@@ -96,9 +96,6 @@
     <t>Requested angle</t>
   </si>
   <si>
-    <t>Set angle</t>
-  </si>
-  <si>
     <t>Truck status 1</t>
   </si>
   <si>
@@ -222,9 +219,6 @@
     <t>Slot 10</t>
   </si>
   <si>
-    <t>Sparse</t>
-  </si>
-  <si>
     <t>ID (Dec)</t>
   </si>
   <si>
@@ -238,6 +232,12 @@
   </si>
   <si>
     <t>Button press</t>
+  </si>
+  <si>
+    <t>ID (HEX)</t>
+  </si>
+  <si>
+    <t>Fault</t>
   </si>
 </sst>
 </file>
@@ -266,7 +266,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="13">
+  <fills count="14">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -336,6 +336,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -352,7 +358,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -365,6 +371,10 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -681,8 +691,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB598DAD-510F-4626-AEEC-E2A56A0E037C}">
   <dimension ref="A1:N16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -755,15 +765,18 @@
         <v>17</v>
       </c>
       <c r="H2" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="I2" s="13" t="s">
         <v>66</v>
       </c>
       <c r="J2" s="9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B3" t="s">
         <v>16</v>
@@ -786,146 +799,146 @@
       <c r="H3" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="2" t="s">
-        <v>19</v>
+      <c r="I3" s="13" t="s">
+        <v>66</v>
       </c>
       <c r="J3" s="9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" t="s">
         <v>21</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="D4" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="6" t="s">
-        <v>24</v>
-      </c>
       <c r="J4" s="9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="D5" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="C5" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>38</v>
-      </c>
       <c r="J5" s="9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="D6" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>43</v>
-      </c>
       <c r="J6" s="9" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" t="s">
         <v>25</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>26</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>27</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>28</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>29</v>
       </c>
-      <c r="G12" t="s">
+      <c r="H12" t="s">
+        <v>56</v>
+      </c>
+      <c r="I12" t="s">
+        <v>57</v>
+      </c>
+      <c r="J12" t="s">
+        <v>58</v>
+      </c>
+      <c r="K12" t="s">
+        <v>59</v>
+      </c>
+      <c r="M12" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="H12" t="s">
-        <v>57</v>
-      </c>
-      <c r="I12" t="s">
-        <v>58</v>
-      </c>
-      <c r="J12" t="s">
-        <v>59</v>
-      </c>
-      <c r="K12" t="s">
-        <v>60</v>
-      </c>
-      <c r="M12" s="5" t="s">
-        <v>31</v>
-      </c>
       <c r="N12" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>47</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="H13" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="I13" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B13" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="E13" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="F13" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="H13" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="I13" s="1" t="s">
+      <c r="J13" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="J13" s="3" t="s">
-        <v>50</v>
-      </c>
       <c r="K13" s="8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M13" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N13" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B14">
         <v>11</v>
@@ -952,26 +965,26 @@
         <v>59</v>
       </c>
       <c r="M14" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="N14" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="M15" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N15" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="M16" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N16" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -985,7 +998,7 @@
   <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -994,140 +1007,181 @@
     <col min="2" max="2" width="10.33203125" customWidth="1"/>
     <col min="3" max="3" width="11.88671875" customWidth="1"/>
     <col min="4" max="4" width="10.5546875" customWidth="1"/>
-    <col min="5" max="6" width="11" customWidth="1"/>
+    <col min="5" max="5" width="11" customWidth="1"/>
+    <col min="6" max="6" width="11.88671875" customWidth="1"/>
     <col min="7" max="7" width="10.44140625" customWidth="1"/>
     <col min="8" max="8" width="11.44140625" customWidth="1"/>
     <col min="10" max="10" width="10.5546875" customWidth="1"/>
+    <col min="11" max="11" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" t="s">
         <v>25</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>26</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>27</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>28</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>29</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I1" t="s">
+        <v>57</v>
+      </c>
+      <c r="J1" t="s">
+        <v>58</v>
+      </c>
+      <c r="K1" t="s">
+        <v>59</v>
+      </c>
+      <c r="M1" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="H1" t="s">
-        <v>57</v>
-      </c>
-      <c r="I1" t="s">
-        <v>58</v>
-      </c>
-      <c r="J1" t="s">
-        <v>59</v>
-      </c>
-      <c r="K1" t="s">
-        <v>60</v>
-      </c>
-      <c r="M1" s="5" t="s">
-        <v>31</v>
-      </c>
       <c r="N1" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="J2" s="3" t="s">
-        <v>50</v>
-      </c>
       <c r="K2" s="8" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>62</v>
-      </c>
-      <c r="B3">
+        <v>60</v>
+      </c>
+      <c r="B3" s="12">
         <v>11</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="12">
         <v>12</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="12">
         <v>13</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="12">
         <v>14</v>
       </c>
-      <c r="G3">
+      <c r="F3" s="12"/>
+      <c r="G3" s="12">
         <v>26</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="12">
         <v>37</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="12">
         <v>48</v>
       </c>
-      <c r="J3">
+      <c r="J3" s="12">
         <v>59</v>
       </c>
+      <c r="K3" s="12"/>
       <c r="M3" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="N3" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B4" s="12" t="str">
+        <f>DEC2HEX(B3)</f>
+        <v>B</v>
+      </c>
+      <c r="C4" s="12" t="str">
+        <f t="shared" ref="C4:K4" si="0">DEC2HEX(C3)</f>
+        <v>C</v>
+      </c>
+      <c r="D4" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v>D</v>
+      </c>
+      <c r="E4" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v>E</v>
+      </c>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v>1A</v>
+      </c>
+      <c r="H4" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="I4" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="J4" s="12" t="str">
+        <f t="shared" si="0"/>
+        <v>3B</v>
+      </c>
+      <c r="K4" s="12"/>
+      <c r="M4" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="N3" s="7" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="M4" s="1" t="s">
-        <v>34</v>
-      </c>
       <c r="N4" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="M5" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="N5" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>